<commit_message>
Setting up local db setup
</commit_message>
<xml_diff>
--- a/model/db_schema.xlsx
+++ b/model/db_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Tom\Documents\Coding\Course\Main\1-Full-Stack Engineer\19-PROJECT_fullstack_ecommerce\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6066EE1C-FB6A-448D-A85E-4F77B9541E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27787EBE-23F0-47AD-BC0F-AA4C4B1BB1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2CF7C30C-1427-407F-B670-830DB5003C08}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>users</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>date_modified</t>
+  </si>
+  <si>
+    <t>uuid</t>
   </si>
 </sst>
 </file>
@@ -558,7 +561,7 @@
   <dimension ref="C2:S14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +610,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>1</v>
@@ -616,7 +619,7 @@
         <v>4</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>21</v>
@@ -625,7 +628,7 @@
         <v>23</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>1</v>
@@ -634,7 +637,7 @@
         <v>4</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="3:19" x14ac:dyDescent="0.25">
@@ -661,7 +664,7 @@
         <v>23</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="Q4" s="1" t="s">
         <v>9</v>
@@ -774,7 +777,7 @@
         <v>23</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>1</v>
@@ -783,7 +786,7 @@
         <v>4</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="3:19" x14ac:dyDescent="0.25">
@@ -794,7 +797,7 @@
         <v>23</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>16</v>

</xml_diff>